<commit_message>
benchmark holding control finish
</commit_message>
<xml_diff>
--- a/Results_ZC/results.xlsx
+++ b/Results_ZC/results.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -28,7 +28,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>No control</t>
+    <t>Holding control</t>
   </si>
 </sst>
 </file>
@@ -411,16 +411,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>2542.949327840155</v>
+        <v>2450.824609460746</v>
       </c>
       <c r="C2">
-        <v>16021.91878786783</v>
+        <v>12623.373108514</v>
       </c>
       <c r="D2">
-        <v>196.009679351595</v>
+        <v>9.034912022317402</v>
       </c>
       <c r="E2">
-        <v>18760.87779505958</v>
+        <v>15083.23262999707</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Analyse in progress create a sheet in one xlsx file
</commit_message>
<xml_diff>
--- a/Results_ZC/results.xlsx
+++ b/Results_ZC/results.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learn\ZCPaper\Collaborative Freight Transport\Model1\Results_ZC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AC1285-79AA-47B0-8361-2B121E08346A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-37605" yWindow="2850" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -34,12 +40,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -47,8 +53,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -94,15 +107,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -144,7 +165,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,9 +197,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,6 +249,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -385,14 +442,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="23.875" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="11.625" customWidth="1"/>
+    <col min="5" max="5" width="11.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -406,24 +472,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>2450.824609460746</v>
+        <v>2450.8246094607462</v>
       </c>
       <c r="C2">
-        <v>12623.373108514</v>
+        <v>12623.373108514001</v>
       </c>
       <c r="D2">
-        <v>9.034912022317402</v>
+        <v>9.0349120223174015</v>
       </c>
       <c r="E2">
         <v>15083.23262999707</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Average_analysis finish, main still be written, exception module
</commit_message>
<xml_diff>
--- a/Results_ZC/results.xlsx
+++ b/Results_ZC/results.xlsx
@@ -1,79 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learn\ZCPaper\Collaborative Freight Transport\Model1\Results_ZC\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AC1285-79AA-47B0-8361-2B121E08346A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-37605" yWindow="2850" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11385" windowWidth="28800" xWindow="-37605" yWindow="2850"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="NC" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>In-vehicle</t>
-  </si>
-  <si>
-    <t>At-stop</t>
-  </si>
-  <si>
-    <t>Extra</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Holding control</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="3"/>
       <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -96,29 +75,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -442,55 +489,128 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="23.875" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="4" max="4" width="11.625" customWidth="1"/>
-    <col min="5" max="5" width="11.75" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="23.875"/>
+    <col customWidth="1" max="2" min="2" width="13.375"/>
+    <col customWidth="1" max="3" min="3" width="12.875"/>
+    <col customWidth="1" max="4" min="4" width="11.625"/>
+    <col customWidth="1" max="5" min="5" width="11.75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>2450.8246094607462</v>
-      </c>
-      <c r="C2">
-        <v>12623.373108514001</v>
-      </c>
-      <c r="D2">
-        <v>9.0349120223174015</v>
-      </c>
-      <c r="E2">
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Holding control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2450.824609460746</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12623.373108514</v>
+      </c>
+      <c r="D2" t="n">
+        <v>9.034912022317402</v>
+      </c>
+      <c r="E2" t="n">
         <v>15083.23262999707</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>No control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2101.086661275402</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12498.70440518066</v>
+      </c>
+      <c r="D2" t="n">
+        <v>141.4698672425732</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14741.26093369863</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
main function modified, change log files to rollover
</commit_message>
<xml_diff>
--- a/Results_ZC/results.xlsx
+++ b/Results_ZC/results.xlsx
@@ -8,6 +8,8 @@
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="NC" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="NC1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="HC" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -613,4 +615,124 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>No control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2101.086661275402</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12498.70440518066</v>
+      </c>
+      <c r="D2" t="n">
+        <v>141.4698672425732</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14741.26093369863</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Holding control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2598.39729042071</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12418.93511103419</v>
+      </c>
+      <c r="D2" t="n">
+        <v>130.1347673362609</v>
+      </c>
+      <c r="E2" t="n">
+        <v>15147.46716879117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
prolong the execution time of holding
</commit_message>
<xml_diff>
--- a/Results_ZC/results.xlsx
+++ b/Results_ZC/results.xlsx
@@ -12,6 +12,11 @@
     <sheet name="HC" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="NC2" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="HC1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="NC3" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="NC4" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="HC2" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="NC5" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="NC6" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -559,6 +564,126 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>No control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2101.086661275402</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12498.70440518066</v>
+      </c>
+      <c r="D2" t="n">
+        <v>141.4698672425732</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14741.26093369863</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>No control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2101.086661275402</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12498.70440518066</v>
+      </c>
+      <c r="D2" t="n">
+        <v>141.4698672425732</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14741.26093369863</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -857,4 +982,184 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>No control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2101.086661275402</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12498.70440518066</v>
+      </c>
+      <c r="D2" t="n">
+        <v>141.4698672425732</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14741.26093369863</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>No control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2101.086661275402</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12498.70440518066</v>
+      </c>
+      <c r="D2" t="n">
+        <v>141.4698672425732</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14741.26093369863</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Holding control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2419.38839847287</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12374.69569905943</v>
+      </c>
+      <c r="D2" t="n">
+        <v>135.403324569714</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14929.48742210201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
weird permission error of txt file
</commit_message>
<xml_diff>
--- a/Results_ZC/results.xlsx
+++ b/Results_ZC/results.xlsx
@@ -19,6 +19,9 @@
     <sheet name="NC6" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="NC7" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="HC3" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="NC8" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="NC9" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="HC4" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -806,7 +809,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -866,7 +869,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -926,7 +929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -969,16 +972,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2598.39729042071</v>
-      </c>
-      <c r="C2" t="n">
-        <v>12418.93511103419</v>
-      </c>
-      <c r="D2" t="n">
-        <v>130.1347673362609</v>
-      </c>
-      <c r="E2" t="n">
-        <v>15147.46716879117</v>
+        <v>2380.504427055388</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12386.98002681963</v>
+      </c>
+      <c r="D2" t="n">
+        <v>132.9256964883952</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14900.41015036342</v>
       </c>
     </row>
   </sheetData>
@@ -986,7 +989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1046,7 +1049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1085,20 +1088,20 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Holding control</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>2338.400307218047</v>
-      </c>
-      <c r="C2" t="n">
-        <v>12390.70170756176</v>
-      </c>
-      <c r="D2" t="n">
-        <v>132.8640879770229</v>
-      </c>
-      <c r="E2" t="n">
-        <v>14861.96610275683</v>
+          <t>No control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2101.086661275402</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12498.70440518066</v>
+      </c>
+      <c r="D2" t="n">
+        <v>141.4698672425732</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14741.26093369863</v>
       </c>
     </row>
   </sheetData>
@@ -1106,7 +1109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1145,20 +1148,20 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>No control</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>2101.086661275402</v>
-      </c>
-      <c r="C2" t="n">
-        <v>12498.70440518066</v>
-      </c>
-      <c r="D2" t="n">
-        <v>141.4698672425732</v>
-      </c>
-      <c r="E2" t="n">
-        <v>14741.26093369863</v>
+          <t>Holding control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2598.39729042071</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12418.93511103419</v>
+      </c>
+      <c r="D2" t="n">
+        <v>130.1347673362609</v>
+      </c>
+      <c r="E2" t="n">
+        <v>15147.46716879117</v>
       </c>
     </row>
   </sheetData>
@@ -1166,7 +1169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1226,7 +1229,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1269,6 +1272,186 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>2338.400307218047</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12390.70170756176</v>
+      </c>
+      <c r="D2" t="n">
+        <v>132.8640879770229</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14861.96610275683</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>No control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2101.086661275402</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12498.70440518066</v>
+      </c>
+      <c r="D2" t="n">
+        <v>141.4698672425732</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14741.26093369863</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>No control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2101.086661275402</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12498.70440518066</v>
+      </c>
+      <c r="D2" t="n">
+        <v>141.4698672425732</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14741.26093369863</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Holding control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>2419.38839847287</v>
       </c>
       <c r="C2" t="n">

</xml_diff>

<commit_message>
hope no bug generated
</commit_message>
<xml_diff>
--- a/Results_ZC/results.xlsx
+++ b/Results_ZC/results.xlsx
@@ -22,6 +22,8 @@
     <sheet name="NC8" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="NC9" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="HC4" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="NC10" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="HC5" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -989,6 +991,126 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>No control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2101.086661275402</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12498.70440518066</v>
+      </c>
+      <c r="D2" t="n">
+        <v>141.4698672425732</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14741.26093369863</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Holding control</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2332.851502775967</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12415.21858912538</v>
+      </c>
+      <c r="D2" t="n">
+        <v>131.7069624993346</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14879.77705440068</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>